<commit_message>
Updated documentation to work towards 16 step mode
</commit_message>
<xml_diff>
--- a/documentation/Mode Cheatsheet.xlsx
+++ b/documentation/Mode Cheatsheet.xlsx
@@ -24,35 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Function Mode</t>
   </si>
   <si>
-    <t>Play</t>
-  </si>
-  <si>
-    <t>Edit</t>
-  </si>
-  <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <t>Mod</t>
-  </si>
-  <si>
-    <t>Mute</t>
-  </si>
-  <si>
-    <t>Save</t>
-  </si>
-  <si>
-    <t>Load</t>
-  </si>
-  <si>
-    <t>Clear</t>
-  </si>
-  <si>
     <t>Mode</t>
   </si>
   <si>
@@ -74,9 +50,6 @@
     <t>Save Mode</t>
   </si>
   <si>
-    <t>Edit Mode</t>
-  </si>
-  <si>
     <t>Note Mode</t>
   </si>
   <si>
@@ -89,16 +62,52 @@
     <t>Jump Mode</t>
   </si>
   <si>
-    <t>Jump4</t>
-  </si>
-  <si>
-    <t>Skip4</t>
-  </si>
-  <si>
     <t>Skip Mode</t>
   </si>
   <si>
-    <t>Quad4</t>
+    <t>PROB</t>
+  </si>
+  <si>
+    <t>RTRIG</t>
+  </si>
+  <si>
+    <t>ACC</t>
+  </si>
+  <si>
+    <t>NOTE</t>
+  </si>
+  <si>
+    <t>MOD</t>
+  </si>
+  <si>
+    <t>JUMP</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>MUTE</t>
+  </si>
+  <si>
+    <t>CLEAR</t>
+  </si>
+  <si>
+    <t>LOAD</t>
+  </si>
+  <si>
+    <t>SAVE</t>
+  </si>
+  <si>
+    <t>PLAY</t>
+  </si>
+  <si>
+    <t>Accent Mode</t>
+  </si>
+  <si>
+    <t>Probability Mode</t>
+  </si>
+  <si>
+    <t>Retrigger Mode</t>
   </si>
 </sst>
 </file>
@@ -130,7 +139,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,13 +166,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -215,13 +218,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -229,20 +239,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -559,262 +559,274 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="3.44140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="7.44140625" style="2" customWidth="1"/>
-    <col min="11" max="14" width="9" style="5" customWidth="1"/>
+    <col min="3" max="10" width="7.44140625" style="1" customWidth="1"/>
+    <col min="11" max="14" width="9" style="2" customWidth="1"/>
     <col min="15" max="19" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
+    <row r="1" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="4"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="10" t="str">
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="9" t="str">
         <f>"01"</f>
         <v>01</v>
       </c>
-      <c r="D3" s="10" t="str">
+      <c r="D3" s="9" t="str">
         <f>"02"</f>
         <v>02</v>
       </c>
-      <c r="E3" s="10" t="str">
+      <c r="E3" s="9" t="str">
         <f>"03"</f>
         <v>03</v>
       </c>
-      <c r="F3" s="10" t="str">
+      <c r="F3" s="9" t="str">
         <f>"04"</f>
         <v>04</v>
       </c>
-      <c r="G3" s="10" t="str">
+      <c r="G3" s="9" t="str">
         <f>"05"</f>
         <v>05</v>
       </c>
-      <c r="H3" s="10" t="str">
+      <c r="H3" s="9" t="str">
         <f>"06"</f>
         <v>06</v>
       </c>
-      <c r="I3" s="10" t="str">
+      <c r="I3" s="9" t="str">
         <f>"07"</f>
         <v>07</v>
       </c>
-      <c r="J3" s="10" t="str">
+      <c r="J3" s="9" t="str">
         <f>"08"</f>
         <v>08</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="7"/>
-      <c r="C4" s="10" t="str">
+      <c r="B4" s="5"/>
+      <c r="C4" s="9" t="str">
         <f>"09"</f>
         <v>09</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>10</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="9">
         <v>11</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="9">
         <v>12</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="9">
         <v>13</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="9">
         <v>14</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="9">
         <v>15</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="9">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="8" t="s">
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-    </row>
-    <row r="8" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="6" t="s">
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-    </row>
-    <row r="9" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-    </row>
-    <row r="10" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-    </row>
-    <row r="11" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-    </row>
-    <row r="12" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-    </row>
-    <row r="13" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-    </row>
-    <row r="14" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-    </row>
-    <row r="15" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E17" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>